<commit_message>
Updated sim_summary table, with backup file
</commit_message>
<xml_diff>
--- a/tables/sim_summary.xlsx
+++ b/tables/sim_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\cdm-science\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D021BA-90D6-4F21-9C3C-CB28D465BF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15217B53-BDED-418E-B746-69C396D58946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{47C7AFC4-A20D-2641-A4AE-6C558E483899}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{47C7AFC4-A20D-2641-A4AE-6C558E483899}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Table</t>
   </si>
@@ -120,12 +120,6 @@
     <t>HCHB</t>
   </si>
   <si>
-    <t>Generation 0</t>
-  </si>
-  <si>
-    <t>2013-2019</t>
-  </si>
-  <si>
     <t>Generation I - rapid</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>Generation I</t>
   </si>
   <si>
-    <t>2020-2021</t>
-  </si>
-  <si>
     <t>Updated with waves, and 20x sediment zones</t>
   </si>
   <si>
@@ -166,6 +157,9 @@
   </si>
   <si>
     <t>AED + HSI + MAG</t>
+  </si>
+  <si>
+    <t>2019-2021</t>
   </si>
 </sst>
 </file>
@@ -544,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C456524-2A98-844E-A03E-E4CD8B8481D9}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -773,21 +767,23 @@
         <v>31</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
@@ -797,24 +793,24 @@
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -826,25 +822,25 @@
         <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -855,54 +851,25 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>